<commit_message>
give non-zero value to amp and sigmaR for testing coverage
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/templates_v16.2/Template_CoMoCOVID-19App_r_v_cpp.xlsx
+++ b/comoOdeCpp/tests/testthat/data/templates_v16.2/Template_CoMoCOVID-19App_r_v_cpp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17895" windowHeight="17580" tabRatio="648" firstSheet="6" activeTab="9"/>
+    <workbookView windowHeight="17850" tabRatio="648" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,6 @@
     <sheet name="Interventions" sheetId="14" r:id="rId10"/>
     <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$36</definedName>
   </definedNames>
@@ -2901,19 +2898,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="33">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2987,11 +2977,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2999,6 +2989,43 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3011,7 +3038,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3026,16 +3053,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3049,60 +3090,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3115,24 +3120,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3208,7 +3198,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3220,43 +3318,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3268,49 +3336,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3322,49 +3348,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3382,7 +3372,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3476,11 +3466,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3509,17 +3540,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3538,184 +3563,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="37" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3726,11 +3716,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3772,77 +3762,77 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3851,14 +3841,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3882,21 +3872,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3918,16 +3908,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3987,39 +3977,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="Cases"/>
-      <sheetName val="Severity-Mortality"/>
-      <sheetName val="Population"/>
-      <sheetName val="Virus Param"/>
-      <sheetName val="Country Area Param"/>
-      <sheetName val="Parameters"/>
-      <sheetName val="Hospitalisation Param"/>
-      <sheetName val="Interventions Param"/>
-      <sheetName val="HIDDEN"/>
-      <sheetName val="Interventions"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4417,8 +4374,8 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -8550,8 +8507,8 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E25"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -8908,7 +8865,7 @@
         <v>177</v>
       </c>
       <c r="B21" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="54" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
not sure what changed in this .xlsx
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/templates_v16.2/Template_CoMoCOVID-19App_r_v_cpp.xlsx
+++ b/comoOdeCpp/tests/testthat/data/templates_v16.2/Template_CoMoCOVID-19App_r_v_cpp.xlsx
@@ -8508,7 +8508,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -8610,7 +8610,7 @@
         <v>146</v>
       </c>
       <c r="B6" s="56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="57" t="s">
         <v>87</v>

</xml_diff>